<commit_message>
Importar asiganacion de equipos, accesorios
</commit_message>
<xml_diff>
--- a/arc/xls/arc_Libro5.xlsx
+++ b/arc/xls/arc_Libro5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvanrivera\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FADE61-E71A-4127-B526-8ECFE7D21B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC937A86-0E49-45D1-A4D3-64CF4AFF2343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="3330" windowWidth="19020" windowHeight="11385" xr2:uid="{83EB8D65-2FC0-49AE-950B-5A8B69ED4B02}"/>
   </bookViews>
@@ -536,9 +536,7 @@
       <c r="E3" s="10">
         <v>15</v>
       </c>
-      <c r="F3" s="10">
-        <v>105</v>
-      </c>
+      <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="1">
         <v>1072642921</v>

</xml_diff>